<commit_message>
refactor: Delete unnecessary data
</commit_message>
<xml_diff>
--- a/src/data_base/BD_Info.xlsx
+++ b/src/data_base/BD_Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iglebov/PycharmProjects/rpa_case/src/data_base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFA92AC-8B76-7541-8FDA-357992068847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3100809-9560-6C47-9E19-D8F4643EE1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="3640" windowWidth="10000" windowHeight="12920" xr2:uid="{36812D43-C824-7B40-A11F-A1DD852D4079}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{36812D43-C824-7B40-A11F-A1DD852D4079}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPANIES_INFO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>companies</t>
+  </si>
+  <si>
+    <t>cases</t>
   </si>
 </sst>
 </file>
@@ -777,7 +780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC65C67E-A4A2-E548-9C56-7F5680BCBE12}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1205,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F58083A-C7E9-4746-A208-8BBF8880E294}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,7 +1223,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="30"/>
+      <c r="A1" s="30" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
       <c r="D1" s="30"/>

</xml_diff>